<commit_message>
Added measurements to the folder
</commit_message>
<xml_diff>
--- a/Temporal_distance_measures_project/mesures_soundtypes_updated.xlsx
+++ b/Temporal_distance_measures_project/mesures_soundtypes_updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d79da97edd0525e/Bureau/Master BEE MNHN/Stage M1 Ecoacoustique/Données/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d79da97edd0525e/Bureau/Ecoacoustic project internship/Acoustic-communities-process-internship/Temporal_distance_measures_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="14_{B4E40D56-3A89-422A-BC6F-2930158930E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BA4629-DD3E-4438-B7C7-D2774E5BFF55}"/>
+  <xr:revisionPtr revIDLastSave="558" documentId="14_{B4E40D56-3A89-422A-BC6F-2930158930E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D22F2F6C-EF8D-44E2-9B6E-9EAAE45981D3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="6456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mesures_soundtypes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="626">
   <si>
     <t>duration</t>
   </si>
@@ -1869,13 +1869,55 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>pace difficult to determinate</t>
+  </si>
+  <si>
+    <t>not sure for pace because duration noted as long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower freq and pace hard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pace hard </t>
+  </si>
+  <si>
+    <t>pace hard</t>
+  </si>
+  <si>
+    <t>can't see the signal</t>
+  </si>
+  <si>
+    <t>duration longer than unit duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all 24 from the same subsample ? </t>
+  </si>
+  <si>
+    <t>duration longer than unit</t>
+  </si>
+  <si>
+    <t>8 supposed to be composed pulse but here no</t>
+  </si>
+  <si>
+    <t>doesn't look like the other 29</t>
+  </si>
+  <si>
+    <t>Potential_category</t>
+  </si>
+  <si>
+    <t>Start to remeasure duration and dom_freq</t>
+  </si>
+  <si>
+    <t>Check again duration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2006,6 +2048,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2733,18 +2781,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I610"/>
+  <dimension ref="A1:J610"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E180" sqref="E180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>610</v>
       </c>
@@ -2770,10 +2819,13 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
+        <v>623</v>
+      </c>
+      <c r="J1" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2797,7 +2849,7 @@
         <v>3.5885167464114835</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2821,7 +2873,7 @@
         <v>4.0128410914927768</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2845,7 +2897,7 @@
         <v>4.0032025620496396</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2869,7 +2921,7 @@
         <v>4.4987146529562985</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2893,7 +2945,7 @@
         <v>4.7846889952153111</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2917,7 +2969,7 @@
         <v>4.057971014492753</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2940,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2963,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2986,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3009,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3032,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3055,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3078,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -3102,7 +3154,7 @@
         <v>15.037593984962406</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3449,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
@@ -3472,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -3496,7 +3548,7 @@
         <v>2.9019152640742889</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -3519,7 +3571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>7</v>
       </c>
@@ -3542,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>7</v>
       </c>
@@ -3566,7 +3618,7 @@
         <v>1.3609145345672291</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
@@ -3589,7 +3641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -3612,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -3625,11 +3677,11 @@
       <c r="D40">
         <v>98</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>8</v>
       </c>
@@ -3652,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>8</v>
       </c>
@@ -3676,7 +3728,7 @@
         <v>2.6455026455026456</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>8</v>
       </c>
@@ -3699,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -3722,11 +3774,11 @@
         <f>7/1</f>
         <v>7</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -3749,11 +3801,11 @@
         <f>4/1</f>
         <v>4</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -3777,7 +3829,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>9</v>
       </c>
@@ -3800,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>9</v>
       </c>
@@ -4202,7 +4254,7 @@
         <v>1.7618927762396175</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>14</v>
       </c>
@@ -4224,11 +4276,11 @@
       <c r="G65">
         <v>0</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>14</v>
       </c>
@@ -4252,7 +4304,7 @@
         <v>20.97902097902098</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>14</v>
       </c>
@@ -4276,7 +4328,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>15</v>
       </c>
@@ -4289,8 +4341,17 @@
       <c r="D68">
         <v>3457</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E68">
+        <v>3262</v>
+      </c>
+      <c r="F68">
+        <v>3707</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>15</v>
       </c>
@@ -4303,8 +4364,20 @@
       <c r="D69">
         <v>7982</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E69">
+        <v>6220</v>
+      </c>
+      <c r="F69">
+        <v>10068</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>15</v>
       </c>
@@ -4317,8 +4390,17 @@
       <c r="D70">
         <v>6437</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E70">
+        <v>6165</v>
+      </c>
+      <c r="F70">
+        <v>8437</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>15</v>
       </c>
@@ -4331,8 +4413,17 @@
       <c r="D71">
         <v>3636</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E71">
+        <v>3520</v>
+      </c>
+      <c r="F71">
+        <v>5411</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>15</v>
       </c>
@@ -4345,8 +4436,18 @@
       <c r="D72">
         <v>9324</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E72">
+        <v>8981</v>
+      </c>
+      <c r="F72">
+        <v>10344</v>
+      </c>
+      <c r="G72">
+        <f>3/2.393</f>
+        <v>1.2536564981195153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>15</v>
       </c>
@@ -4359,8 +4460,17 @@
       <c r="D73">
         <v>8201</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>6525</v>
+      </c>
+      <c r="F73">
+        <v>10183</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>16</v>
       </c>
@@ -4373,8 +4483,18 @@
       <c r="D74">
         <v>6937</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E74">
+        <v>6416</v>
+      </c>
+      <c r="F74">
+        <v>9544</v>
+      </c>
+      <c r="G74">
+        <f>16/1.412</f>
+        <v>11.3314447592068</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>16</v>
       </c>
@@ -4387,8 +4507,21 @@
       <c r="D75">
         <v>7997</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E75">
+        <v>6285</v>
+      </c>
+      <c r="F75">
+        <v>9050</v>
+      </c>
+      <c r="G75">
+        <f>10/0.846</f>
+        <v>11.82033096926714</v>
+      </c>
+      <c r="J75" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>16</v>
       </c>
@@ -4401,8 +4534,18 @@
       <c r="D76">
         <v>8982</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E76">
+        <v>8772</v>
+      </c>
+      <c r="F76">
+        <v>9973</v>
+      </c>
+      <c r="G76">
+        <f>5/1.747</f>
+        <v>2.8620492272467084</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>16</v>
       </c>
@@ -4415,8 +4558,18 @@
       <c r="D77">
         <v>10553</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E77">
+        <v>7910</v>
+      </c>
+      <c r="F77">
+        <v>18634</v>
+      </c>
+      <c r="G77">
+        <f>10/0.463</f>
+        <v>21.598272138228939</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>16</v>
       </c>
@@ -4429,8 +4582,18 @@
       <c r="D78">
         <v>2594</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E78">
+        <v>643</v>
+      </c>
+      <c r="F78">
+        <v>5608</v>
+      </c>
+      <c r="G78">
+        <f>13/1.585</f>
+        <v>8.2018927444794958</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>16</v>
       </c>
@@ -4443,8 +4606,18 @@
       <c r="D79">
         <v>8100</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E79">
+        <v>7150</v>
+      </c>
+      <c r="F79">
+        <v>9516</v>
+      </c>
+      <c r="G79">
+        <f>8/0.265</f>
+        <v>30.188679245283016</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>17</v>
       </c>
@@ -4457,8 +4630,18 @@
       <c r="D80">
         <v>13491</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E80">
+        <v>12632</v>
+      </c>
+      <c r="F80">
+        <v>16619</v>
+      </c>
+      <c r="G80">
+        <f>10/0.693</f>
+        <v>14.430014430014431</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>17</v>
       </c>
@@ -4471,8 +4654,21 @@
       <c r="D81">
         <v>15231</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E81">
+        <v>11900</v>
+      </c>
+      <c r="F81">
+        <v>19785</v>
+      </c>
+      <c r="G81">
+        <f>4/0.334</f>
+        <v>11.976047904191615</v>
+      </c>
+      <c r="J81" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>17</v>
       </c>
@@ -4485,8 +4681,20 @@
       <c r="D82">
         <v>8988</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E82">
+        <v>8770</v>
+      </c>
+      <c r="F82">
+        <v>10000</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>17</v>
       </c>
@@ -4499,8 +4707,17 @@
       <c r="D83">
         <v>13284</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E83">
+        <v>10950</v>
+      </c>
+      <c r="F83">
+        <v>14100</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>17</v>
       </c>
@@ -4513,8 +4730,18 @@
       <c r="D84">
         <v>14353</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E84">
+        <v>12030</v>
+      </c>
+      <c r="F84">
+        <v>15265</v>
+      </c>
+      <c r="G84">
+        <f>6/0.192</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>17</v>
       </c>
@@ -4527,8 +4754,17 @@
       <c r="D85">
         <v>7035</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E85">
+        <v>6764</v>
+      </c>
+      <c r="F85">
+        <v>7934</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>18</v>
       </c>
@@ -4541,8 +4777,18 @@
       <c r="D86">
         <v>1468</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E86">
+        <v>386</v>
+      </c>
+      <c r="F86">
+        <v>14676</v>
+      </c>
+      <c r="G86">
+        <f>4/0.17</f>
+        <v>23.52941176470588</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>19</v>
       </c>
@@ -4555,8 +4801,17 @@
       <c r="D87">
         <v>2712</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E87">
+        <v>2178</v>
+      </c>
+      <c r="F87">
+        <v>2862</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>19</v>
       </c>
@@ -4569,8 +4824,18 @@
       <c r="D88">
         <v>951</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E88">
+        <v>138</v>
+      </c>
+      <c r="F88">
+        <v>5367</v>
+      </c>
+      <c r="G88">
+        <f>10/0.472</f>
+        <v>21.186440677966104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>19</v>
       </c>
@@ -4583,8 +4848,18 @@
       <c r="D89">
         <v>1877</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E89">
+        <v>265</v>
+      </c>
+      <c r="F89">
+        <v>2779</v>
+      </c>
+      <c r="G89">
+        <f>7/0.495</f>
+        <v>14.141414141414142</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>19</v>
       </c>
@@ -4597,8 +4872,20 @@
       <c r="D90">
         <v>4245</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E90">
+        <v>3510</v>
+      </c>
+      <c r="F90">
+        <v>7274</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="J90" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>19</v>
       </c>
@@ -4611,8 +4898,17 @@
       <c r="D91">
         <v>2285</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E91">
+        <v>873</v>
+      </c>
+      <c r="F91">
+        <v>3939</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>19</v>
       </c>
@@ -4625,8 +4921,18 @@
       <c r="D92">
         <v>1354</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E92">
+        <v>110</v>
+      </c>
+      <c r="F92">
+        <v>10401</v>
+      </c>
+      <c r="G92">
+        <f>8/0.304</f>
+        <v>26.315789473684212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>20</v>
       </c>
@@ -4639,8 +4945,18 @@
       <c r="D93">
         <v>13682</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E93">
+        <v>819</v>
+      </c>
+      <c r="F93">
+        <v>16144</v>
+      </c>
+      <c r="G93">
+        <f>5/0.276</f>
+        <v>18.115942028985504</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>21</v>
       </c>
@@ -4653,8 +4969,18 @@
       <c r="D94">
         <v>355</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E94">
+        <v>187</v>
+      </c>
+      <c r="F94">
+        <v>570</v>
+      </c>
+      <c r="G94">
+        <f>2/1.853</f>
+        <v>1.0793308148947653</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>21</v>
       </c>
@@ -4667,8 +4993,11 @@
       <c r="D95">
         <v>375</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J95" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>21</v>
       </c>
@@ -4681,8 +5010,18 @@
       <c r="D96">
         <v>2702</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E96">
+        <v>270</v>
+      </c>
+      <c r="F96">
+        <v>7862</v>
+      </c>
+      <c r="G96">
+        <f>9/0.417</f>
+        <v>21.582733812949641</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>21</v>
       </c>
@@ -4695,8 +5034,18 @@
       <c r="D97">
         <v>5541</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>10474</v>
+      </c>
+      <c r="G97">
+        <f>10/0.6</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>21</v>
       </c>
@@ -4709,8 +5058,17 @@
       <c r="D98">
         <v>131</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>720</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>21</v>
       </c>
@@ -4723,8 +5081,17 @@
       <c r="D99">
         <v>208</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>4929</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>22</v>
       </c>
@@ -4737,8 +5104,18 @@
       <c r="D100">
         <v>2381</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E100">
+        <v>1188</v>
+      </c>
+      <c r="F100">
+        <v>22050</v>
+      </c>
+      <c r="G100">
+        <f>7/3.389</f>
+        <v>2.0655060489820007</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>22</v>
       </c>
@@ -4751,8 +5128,18 @@
       <c r="D101">
         <v>3543</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E101">
+        <v>2942</v>
+      </c>
+      <c r="F101">
+        <v>3961</v>
+      </c>
+      <c r="G101">
+        <f>4/0.29</f>
+        <v>13.793103448275863</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>22</v>
       </c>
@@ -4765,8 +5152,18 @@
       <c r="D102">
         <v>10942</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E102">
+        <v>1679</v>
+      </c>
+      <c r="F102">
+        <v>22050</v>
+      </c>
+      <c r="G102">
+        <f>4/1.427</f>
+        <v>2.8030833917309037</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>22</v>
       </c>
@@ -4779,8 +5176,21 @@
       <c r="D103">
         <v>904</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E103">
+        <v>88</v>
+      </c>
+      <c r="F103">
+        <v>10034</v>
+      </c>
+      <c r="G103">
+        <f>7/0.303</f>
+        <v>23.102310231023104</v>
+      </c>
+      <c r="J103" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>22</v>
       </c>
@@ -4793,8 +5203,18 @@
       <c r="D104">
         <v>3918</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E104">
+        <v>3374</v>
+      </c>
+      <c r="F104">
+        <v>15244</v>
+      </c>
+      <c r="G104">
+        <f>4/0.19</f>
+        <v>21.05263157894737</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>22</v>
       </c>
@@ -4807,8 +5227,18 @@
       <c r="D105">
         <v>5271</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E105">
+        <v>240</v>
+      </c>
+      <c r="F105">
+        <v>15117</v>
+      </c>
+      <c r="G105">
+        <f>3/2.811</f>
+        <v>1.0672358591248665</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>23</v>
       </c>
@@ -4821,8 +5251,18 @@
       <c r="D106">
         <v>383</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>944</v>
+      </c>
+      <c r="G106">
+        <f>4/0.165</f>
+        <v>24.242424242424242</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>23</v>
       </c>
@@ -4835,8 +5275,18 @@
       <c r="D107">
         <v>1080</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E107">
+        <v>526</v>
+      </c>
+      <c r="F107">
+        <v>4222</v>
+      </c>
+      <c r="G107">
+        <f>5/0.238</f>
+        <v>21.008403361344538</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>23</v>
       </c>
@@ -4849,8 +5299,18 @@
       <c r="D108">
         <v>1878</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E108">
+        <v>1527</v>
+      </c>
+      <c r="F108">
+        <v>2763</v>
+      </c>
+      <c r="G108">
+        <f>2/0.77</f>
+        <v>2.5974025974025974</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>23</v>
       </c>
@@ -4863,8 +5323,18 @@
       <c r="D109">
         <v>1704</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E109">
+        <v>1438</v>
+      </c>
+      <c r="F109">
+        <v>2742</v>
+      </c>
+      <c r="G109">
+        <f>2/1.362</f>
+        <v>1.4684287812041115</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>23</v>
       </c>
@@ -4877,8 +5347,17 @@
       <c r="D110">
         <v>1316</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E110">
+        <v>1178</v>
+      </c>
+      <c r="F110">
+        <v>3514</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>23</v>
       </c>
@@ -4891,8 +5370,17 @@
       <c r="D111">
         <v>1210</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E111">
+        <v>533</v>
+      </c>
+      <c r="F111">
+        <v>1274</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>24</v>
       </c>
@@ -4905,8 +5393,21 @@
       <c r="D112">
         <v>13156</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E112">
+        <v>10647</v>
+      </c>
+      <c r="F112">
+        <v>22050</v>
+      </c>
+      <c r="G112">
+        <f>12/1.802</f>
+        <v>6.6592674805771361</v>
+      </c>
+      <c r="J112" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>24</v>
       </c>
@@ -4919,8 +5420,21 @@
       <c r="D113">
         <v>13060</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E113">
+        <v>10647</v>
+      </c>
+      <c r="F113">
+        <v>22050</v>
+      </c>
+      <c r="G113">
+        <f t="shared" ref="G113:G117" si="0">12/1.802</f>
+        <v>6.6592674805771361</v>
+      </c>
+      <c r="J113" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>24</v>
       </c>
@@ -4933,8 +5447,21 @@
       <c r="D114">
         <v>12762</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E114">
+        <v>10647</v>
+      </c>
+      <c r="F114">
+        <v>22050</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="0"/>
+        <v>6.6592674805771361</v>
+      </c>
+      <c r="J114" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>24</v>
       </c>
@@ -4947,8 +5474,21 @@
       <c r="D115">
         <v>13309</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E115">
+        <v>10647</v>
+      </c>
+      <c r="F115">
+        <v>22050</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="0"/>
+        <v>6.6592674805771361</v>
+      </c>
+      <c r="J115" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>24</v>
       </c>
@@ -4961,8 +5501,21 @@
       <c r="D116">
         <v>13506</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E116">
+        <v>10647</v>
+      </c>
+      <c r="F116">
+        <v>22050</v>
+      </c>
+      <c r="G116">
+        <f t="shared" si="0"/>
+        <v>6.6592674805771361</v>
+      </c>
+      <c r="J116" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>24</v>
       </c>
@@ -4975,8 +5528,21 @@
       <c r="D117">
         <v>13328</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E117">
+        <v>10647</v>
+      </c>
+      <c r="F117">
+        <v>22050</v>
+      </c>
+      <c r="G117">
+        <f t="shared" si="0"/>
+        <v>6.6592674805771361</v>
+      </c>
+      <c r="J117" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>25</v>
       </c>
@@ -4989,8 +5555,18 @@
       <c r="D118">
         <v>8796</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E118">
+        <v>4524</v>
+      </c>
+      <c r="F118">
+        <v>11464</v>
+      </c>
+      <c r="G118">
+        <f>2/0.062</f>
+        <v>32.258064516129032</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>25</v>
       </c>
@@ -5003,8 +5579,18 @@
       <c r="D119">
         <v>13997</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E119">
+        <v>621</v>
+      </c>
+      <c r="F119">
+        <v>17922</v>
+      </c>
+      <c r="G119">
+        <f>3/0.211</f>
+        <v>14.218009478672986</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>25</v>
       </c>
@@ -5017,8 +5603,17 @@
       <c r="D120">
         <v>15685</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E120">
+        <v>8042</v>
+      </c>
+      <c r="F120">
+        <v>19574</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>25</v>
       </c>
@@ -5031,8 +5626,17 @@
       <c r="D121">
         <v>11280</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E121">
+        <v>1968</v>
+      </c>
+      <c r="F121">
+        <v>12235</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>25</v>
       </c>
@@ -5045,8 +5649,17 @@
       <c r="D122">
         <v>8389</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E122">
+        <v>5779</v>
+      </c>
+      <c r="F122">
+        <v>13900</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>25</v>
       </c>
@@ -5059,8 +5672,17 @@
       <c r="D123">
         <v>14528</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>15401</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>26</v>
       </c>
@@ -5073,8 +5695,18 @@
       <c r="D124">
         <v>4703</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E124">
+        <v>143</v>
+      </c>
+      <c r="F124">
+        <v>22050</v>
+      </c>
+      <c r="G124">
+        <f>4/0.279</f>
+        <v>14.336917562724013</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>26</v>
       </c>
@@ -5087,8 +5719,18 @@
       <c r="D125">
         <v>2027</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E125">
+        <v>81</v>
+      </c>
+      <c r="F125">
+        <v>4235</v>
+      </c>
+      <c r="G125">
+        <f>10/1.087</f>
+        <v>9.1996320147194108</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>26</v>
       </c>
@@ -5101,8 +5743,18 @@
       <c r="D126">
         <v>1605</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E126">
+        <v>60</v>
+      </c>
+      <c r="F126">
+        <v>5817</v>
+      </c>
+      <c r="G126">
+        <f>4/0.389</f>
+        <v>10.282776349614396</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>27</v>
       </c>
@@ -5115,8 +5767,21 @@
       <c r="D127">
         <v>9359</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E127">
+        <v>7719</v>
+      </c>
+      <c r="F127">
+        <v>11286</v>
+      </c>
+      <c r="G127">
+        <f>6/0.175</f>
+        <v>34.285714285714285</v>
+      </c>
+      <c r="J127" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>27</v>
       </c>
@@ -5129,8 +5794,20 @@
       <c r="D128">
         <v>9372</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E128">
+        <v>7588</v>
+      </c>
+      <c r="F128">
+        <v>12081</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="J128" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>27</v>
       </c>
@@ -5143,8 +5820,18 @@
       <c r="D129">
         <v>10392</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E129">
+        <v>7671</v>
+      </c>
+      <c r="F129">
+        <v>11386</v>
+      </c>
+      <c r="G129">
+        <f>7/0.227</f>
+        <v>30.837004405286343</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>27</v>
       </c>
@@ -5157,8 +5844,18 @@
       <c r="D130">
         <v>10392</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E130">
+        <v>8560</v>
+      </c>
+      <c r="F130">
+        <v>11397</v>
+      </c>
+      <c r="G130">
+        <f>8/0.25</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>27</v>
       </c>
@@ -5171,8 +5868,18 @@
       <c r="D131">
         <v>8433</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E131">
+        <v>6794</v>
+      </c>
+      <c r="F131">
+        <v>10047</v>
+      </c>
+      <c r="G131">
+        <f>9/0.33</f>
+        <v>27.27272727272727</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>27</v>
       </c>
@@ -5185,8 +5892,18 @@
       <c r="D132">
         <v>9596</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E132">
+        <v>7358</v>
+      </c>
+      <c r="F132">
+        <v>10936</v>
+      </c>
+      <c r="G132">
+        <f>11/0.25</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>28</v>
       </c>
@@ -5199,8 +5916,20 @@
       <c r="D133">
         <v>9049</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E133">
+        <v>3155</v>
+      </c>
+      <c r="F133">
+        <v>19867</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="J133" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>28</v>
       </c>
@@ -5213,8 +5942,20 @@
       <c r="D134">
         <v>9011</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E134">
+        <v>4332</v>
+      </c>
+      <c r="F134">
+        <v>19498</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+      <c r="J134" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>28</v>
       </c>
@@ -5227,8 +5968,20 @@
       <c r="D135">
         <v>9076</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E135">
+        <v>3924</v>
+      </c>
+      <c r="F135">
+        <v>19771</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+      <c r="J135" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>28</v>
       </c>
@@ -5241,8 +5994,20 @@
       <c r="D136">
         <v>9062</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E136">
+        <v>3087</v>
+      </c>
+      <c r="F136">
+        <v>19868</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+      <c r="J136" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>29</v>
       </c>
@@ -5255,8 +6020,18 @@
       <c r="D137">
         <v>3463</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E137">
+        <v>521</v>
+      </c>
+      <c r="F137">
+        <v>8902</v>
+      </c>
+      <c r="G137">
+        <f>6/3.478</f>
+        <v>1.7251293847038527</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>29</v>
       </c>
@@ -5269,8 +6044,18 @@
       <c r="D138">
         <v>2415</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E138">
+        <v>1723</v>
+      </c>
+      <c r="F138">
+        <v>6539</v>
+      </c>
+      <c r="G138">
+        <f>5/0.129</f>
+        <v>38.759689922480618</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>29</v>
       </c>
@@ -5283,8 +6068,18 @@
       <c r="D139">
         <v>3294</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E139">
+        <v>2558</v>
+      </c>
+      <c r="F139">
+        <v>9946</v>
+      </c>
+      <c r="G139">
+        <f>9/0.2</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>29</v>
       </c>
@@ -5297,8 +6092,18 @@
       <c r="D140">
         <v>7999</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E140">
+        <v>1911</v>
+      </c>
+      <c r="F140">
+        <v>10026</v>
+      </c>
+      <c r="G140">
+        <f>5/0.122</f>
+        <v>40.983606557377051</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>29</v>
       </c>
@@ -5311,8 +6116,18 @@
       <c r="D141">
         <v>5557</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E141">
+        <v>287</v>
+      </c>
+      <c r="F141">
+        <v>10023</v>
+      </c>
+      <c r="G141">
+        <f>7/0.28</f>
+        <v>24.999999999999996</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>29</v>
       </c>
@@ -5325,8 +6140,20 @@
       <c r="D142">
         <v>5668</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E142">
+        <v>3441</v>
+      </c>
+      <c r="F142">
+        <v>9404</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="J142" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>30</v>
       </c>
@@ -5339,8 +6166,18 @@
       <c r="D143">
         <v>9150</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E143">
+        <v>3932</v>
+      </c>
+      <c r="F143">
+        <v>9551</v>
+      </c>
+      <c r="G143">
+        <f>2/0.038</f>
+        <v>52.631578947368425</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>30</v>
       </c>
@@ -5353,8 +6190,18 @@
       <c r="D144">
         <v>9223</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E144">
+        <v>3901</v>
+      </c>
+      <c r="F144">
+        <v>9551</v>
+      </c>
+      <c r="G144">
+        <f>2/0.049</f>
+        <v>40.816326530612244</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>30</v>
       </c>
@@ -5367,8 +6214,18 @@
       <c r="D145">
         <v>9015</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E145">
+        <v>3823</v>
+      </c>
+      <c r="F145">
+        <v>9546</v>
+      </c>
+      <c r="G145">
+        <f>2/0.043</f>
+        <v>46.511627906976749</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>31</v>
       </c>
@@ -5381,8 +6238,18 @@
       <c r="D146">
         <v>3449</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E146">
+        <v>2612</v>
+      </c>
+      <c r="F146">
+        <v>4876</v>
+      </c>
+      <c r="G146">
+        <f>4/1.545</f>
+        <v>2.5889967637540456</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>31</v>
       </c>
@@ -5395,8 +6262,18 @@
       <c r="D147">
         <v>3335</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E147">
+        <v>2378</v>
+      </c>
+      <c r="F147">
+        <v>4465</v>
+      </c>
+      <c r="G147">
+        <f>5/1.502</f>
+        <v>3.3288948069241013</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>31</v>
       </c>
@@ -5409,8 +6286,18 @@
       <c r="D148">
         <v>3402</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E148">
+        <v>2571</v>
+      </c>
+      <c r="F148">
+        <v>4329</v>
+      </c>
+      <c r="G148">
+        <f>5/1.746</f>
+        <v>2.86368843069874</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>31</v>
       </c>
@@ -5423,8 +6310,18 @@
       <c r="D149">
         <v>3262</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E149">
+        <v>2901</v>
+      </c>
+      <c r="F149">
+        <v>3656</v>
+      </c>
+      <c r="G149">
+        <f>4/1.634</f>
+        <v>2.4479804161566707</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>31</v>
       </c>
@@ -5437,8 +6334,18 @@
       <c r="D150">
         <v>3423</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E150">
+        <v>2288</v>
+      </c>
+      <c r="F150">
+        <v>4785</v>
+      </c>
+      <c r="G150">
+        <f>4/1.416</f>
+        <v>2.8248587570621471</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>31</v>
       </c>
@@ -5451,8 +6358,18 @@
       <c r="D151">
         <v>4081</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E151">
+        <v>2212</v>
+      </c>
+      <c r="F151">
+        <v>4627</v>
+      </c>
+      <c r="G151">
+        <f>3/1.114</f>
+        <v>2.6929982046678633</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>32</v>
       </c>
@@ -5465,8 +6382,17 @@
       <c r="D152">
         <v>15302</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E152">
+        <v>5584</v>
+      </c>
+      <c r="F152">
+        <v>21474</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>32</v>
       </c>
@@ -5479,8 +6405,17 @@
       <c r="D153">
         <v>15053</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E153">
+        <v>2432</v>
+      </c>
+      <c r="F153">
+        <v>16540</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>33</v>
       </c>
@@ -5493,8 +6428,18 @@
       <c r="D154">
         <v>15128</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E154">
+        <v>12355</v>
+      </c>
+      <c r="F154">
+        <v>15843</v>
+      </c>
+      <c r="G154">
+        <f>2/0.304</f>
+        <v>6.5789473684210531</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>33</v>
       </c>
@@ -5507,8 +6452,17 @@
       <c r="D155">
         <v>8931</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E155">
+        <v>7595</v>
+      </c>
+      <c r="F155">
+        <v>9878</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>33</v>
       </c>
@@ -5521,8 +6475,18 @@
       <c r="D156">
         <v>7934</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E156">
+        <v>7843</v>
+      </c>
+      <c r="F156">
+        <v>15450</v>
+      </c>
+      <c r="G156">
+        <f>3/5.275</f>
+        <v>0.56872037914691942</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>33</v>
       </c>
@@ -5535,8 +6499,18 @@
       <c r="D157">
         <v>9949</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E157">
+        <v>9285</v>
+      </c>
+      <c r="F157">
+        <v>17760</v>
+      </c>
+      <c r="G157">
+        <f>5/7.453</f>
+        <v>0.67087079028579089</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>33</v>
       </c>
@@ -5549,8 +6523,18 @@
       <c r="D158">
         <v>11247</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E158">
+        <v>6397</v>
+      </c>
+      <c r="F158">
+        <v>16641</v>
+      </c>
+      <c r="G158">
+        <f>7/7.34</f>
+        <v>0.9536784741144414</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>33</v>
       </c>
@@ -5563,8 +6547,17 @@
       <c r="D159">
         <v>5443</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E159">
+        <v>3633</v>
+      </c>
+      <c r="F159">
+        <v>7071</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>34</v>
       </c>
@@ -5575,10 +6568,26 @@
         <v>0.54900000000000004</v>
       </c>
       <c r="D160">
-        <v>5360</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5446</v>
+      </c>
+      <c r="E160">
+        <v>4733</v>
+      </c>
+      <c r="F160">
+        <v>7756</v>
+      </c>
+      <c r="G160">
+        <f>2/1.358</f>
+        <v>1.4727540500736376</v>
+      </c>
+      <c r="I160">
+        <v>5</v>
+      </c>
+      <c r="J160" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>34</v>
       </c>
@@ -5586,13 +6595,26 @@
         <v>154</v>
       </c>
       <c r="C161">
-        <v>1.921</v>
+        <v>0.1</v>
       </c>
       <c r="D161">
-        <v>10060</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9994</v>
+      </c>
+      <c r="E161">
+        <v>8823</v>
+      </c>
+      <c r="F161">
+        <v>13982</v>
+      </c>
+      <c r="G161">
+        <f>2/0.222</f>
+        <v>9.0090090090090094</v>
+      </c>
+      <c r="I161">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>34</v>
       </c>
@@ -5600,13 +6622,26 @@
         <v>155</v>
       </c>
       <c r="C162">
-        <v>1.296</v>
+        <v>0.106</v>
       </c>
       <c r="D162">
-        <v>6840</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7016</v>
+      </c>
+      <c r="E162">
+        <v>6547</v>
+      </c>
+      <c r="F162">
+        <v>8826</v>
+      </c>
+      <c r="G162">
+        <f>3/0.319</f>
+        <v>9.4043887147335425</v>
+      </c>
+      <c r="I162">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>34</v>
       </c>
@@ -5614,13 +6649,25 @@
         <v>156</v>
       </c>
       <c r="C163">
-        <v>0.23799999999999999</v>
+        <v>0.151</v>
       </c>
       <c r="D163">
         <v>9228</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E163">
+        <v>8356</v>
+      </c>
+      <c r="F163">
+        <v>11246</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="I163">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>34</v>
       </c>
@@ -5628,13 +6675,26 @@
         <v>157</v>
       </c>
       <c r="C164">
-        <v>1.028</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="D164">
-        <v>10144</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10162</v>
+      </c>
+      <c r="E164">
+        <v>9412</v>
+      </c>
+      <c r="F164">
+        <v>12838</v>
+      </c>
+      <c r="G164">
+        <f>3/6.881</f>
+        <v>0.43598314198517657</v>
+      </c>
+      <c r="I164">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>34</v>
       </c>
@@ -5645,10 +6705,22 @@
         <v>0.82899999999999996</v>
       </c>
       <c r="D165">
-        <v>9580</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9675</v>
+      </c>
+      <c r="E165">
+        <v>6836</v>
+      </c>
+      <c r="F165">
+        <v>12088</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="I165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>35</v>
       </c>
@@ -5656,13 +6728,29 @@
         <v>159</v>
       </c>
       <c r="C166">
-        <v>6.5000000000000002E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D166">
-        <v>6773</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3167</v>
+      </c>
+      <c r="E166">
+        <v>525</v>
+      </c>
+      <c r="F166">
+        <v>8876</v>
+      </c>
+      <c r="G166">
+        <f>7/0.276</f>
+        <v>25.362318840579707</v>
+      </c>
+      <c r="I166">
+        <v>4</v>
+      </c>
+      <c r="J166" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>35</v>
       </c>
@@ -5670,13 +6758,26 @@
         <v>160</v>
       </c>
       <c r="C167">
-        <v>7.4999999999999997E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="D167">
-        <v>8935</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5112</v>
+      </c>
+      <c r="E167">
+        <v>1011</v>
+      </c>
+      <c r="F167">
+        <v>13288</v>
+      </c>
+      <c r="G167">
+        <f>8/0.317</f>
+        <v>25.236593059936908</v>
+      </c>
+      <c r="I167">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>35</v>
       </c>
@@ -5684,13 +6785,25 @@
         <v>161</v>
       </c>
       <c r="C168">
-        <v>0.05</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="D168">
         <v>6351</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E168">
+        <v>3774</v>
+      </c>
+      <c r="F168">
+        <v>8509</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="I168">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>35</v>
       </c>
@@ -5698,13 +6811,25 @@
         <v>162</v>
       </c>
       <c r="C169">
-        <v>0.14099999999999999</v>
+        <v>0.155</v>
       </c>
       <c r="D169">
-        <v>11885</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11906</v>
+      </c>
+      <c r="E169">
+        <v>7348</v>
+      </c>
+      <c r="F169">
+        <v>16613</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+      <c r="I169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>35</v>
       </c>
@@ -5712,13 +6837,25 @@
         <v>163</v>
       </c>
       <c r="C170">
-        <v>2.5999999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D170">
-        <v>5610</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5587</v>
+      </c>
+      <c r="E170">
+        <v>4810</v>
+      </c>
+      <c r="F170">
+        <v>8413</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="I170">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>35</v>
       </c>
@@ -5726,13 +6863,26 @@
         <v>164</v>
       </c>
       <c r="C171">
-        <v>5.8999999999999997E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D171">
-        <v>5395</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9951</v>
+      </c>
+      <c r="E171">
+        <v>9559</v>
+      </c>
+      <c r="F171">
+        <v>13015</v>
+      </c>
+      <c r="G171">
+        <f>2/0.059</f>
+        <v>33.898305084745765</v>
+      </c>
+      <c r="I171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>36</v>
       </c>
@@ -5740,13 +6890,25 @@
         <v>165</v>
       </c>
       <c r="C172">
-        <v>0.91</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="D172">
-        <v>6245</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6216</v>
+      </c>
+      <c r="E172">
+        <v>193</v>
+      </c>
+      <c r="F172">
+        <v>9648</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="I172">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>37</v>
       </c>
@@ -5754,13 +6916,25 @@
         <v>166</v>
       </c>
       <c r="C173">
-        <v>0.123</v>
+        <v>0.1</v>
       </c>
       <c r="D173">
         <v>9406</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E173">
+        <v>9199</v>
+      </c>
+      <c r="F173">
+        <v>13062</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="I173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>37</v>
       </c>
@@ -5768,13 +6942,25 @@
         <v>167</v>
       </c>
       <c r="C174">
-        <v>6.5000000000000002E-2</v>
+        <v>0.1</v>
       </c>
       <c r="D174">
-        <v>8930</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8641</v>
+      </c>
+      <c r="E174">
+        <v>4638</v>
+      </c>
+      <c r="F174">
+        <v>11121</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="I174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>37</v>
       </c>
@@ -5787,8 +6973,21 @@
       <c r="D175">
         <v>5730</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E175">
+        <v>1680</v>
+      </c>
+      <c r="F175">
+        <v>13993</v>
+      </c>
+      <c r="G175">
+        <f>3/0.227</f>
+        <v>13.215859030837004</v>
+      </c>
+      <c r="I175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>37</v>
       </c>
@@ -5799,10 +6998,23 @@
         <v>3.9E-2</v>
       </c>
       <c r="D176">
-        <v>10137</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10231</v>
+      </c>
+      <c r="E176">
+        <v>9102</v>
+      </c>
+      <c r="F176">
+        <v>11245</v>
+      </c>
+      <c r="G176">
+        <f>5/5.758</f>
+        <v>0.86835706842653704</v>
+      </c>
+      <c r="I176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>37</v>
       </c>
@@ -5810,13 +7022,25 @@
         <v>170</v>
       </c>
       <c r="C177">
-        <v>2.5000000000000001E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="D177">
-        <v>11846</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11618</v>
+      </c>
+      <c r="E177">
+        <v>9279</v>
+      </c>
+      <c r="F177">
+        <v>14667</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+      <c r="I177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>37</v>
       </c>
@@ -5827,10 +7051,22 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D178">
-        <v>15150</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14213</v>
+      </c>
+      <c r="E178">
+        <v>13183</v>
+      </c>
+      <c r="F178">
+        <v>16230</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="I178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>38</v>
       </c>
@@ -5844,7 +7080,7 @@
         <v>13290</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>38</v>
       </c>
@@ -5858,7 +7094,7 @@
         <v>11688</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>38</v>
       </c>
@@ -5872,7 +7108,7 @@
         <v>11443</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>38</v>
       </c>
@@ -5886,7 +7122,7 @@
         <v>10958</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>38</v>
       </c>
@@ -5900,7 +7136,7 @@
         <v>13371</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>38</v>
       </c>
@@ -5914,7 +7150,7 @@
         <v>11323</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>39</v>
       </c>
@@ -5928,7 +7164,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>39</v>
       </c>
@@ -5942,7 +7178,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>39</v>
       </c>
@@ -5956,7 +7192,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>39</v>
       </c>
@@ -5970,7 +7206,7 @@
         <v>2548</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>39</v>
       </c>
@@ -5984,7 +7220,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>39</v>
       </c>
@@ -5998,7 +7234,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>40</v>
       </c>
@@ -6012,7 +7248,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>40</v>
       </c>
@@ -11879,6 +13115,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>